<commit_message>
fixed bug with duplicates
[x] reran all analysis
[x] updated word doc
</commit_message>
<xml_diff>
--- a/Part_2_tables/cited_by_min_max_med.xlsx
+++ b/Part_2_tables/cited_by_min_max_med.xlsx
@@ -465,10 +465,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>4.069441664998999</v>
+        <v>4.07188626351622</v>
       </c>
       <c r="C3" t="n">
-        <v>5.519011406844107</v>
+        <v>5.52232679215058</v>
       </c>
     </row>
     <row r="4">

</xml_diff>